<commit_message>
Projekt zaliczeniowy wraz z plikami
</commit_message>
<xml_diff>
--- a/Malzenstwa.xlsx
+++ b/Malzenstwa.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="770">
   <si>
     <t>Kategoria:</t>
   </si>
@@ -36,10 +36,10 @@
     <t>Podgrupa:</t>
   </si>
   <si>
-    <t>Małżeństwa zawarte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Małżeństwa zawarte w ciągu roku;  Źródłem informacji o małżeństwach jest dla GUS sprawozdawczość urzędów stanu cywilnego w postaci formularzy statystycznych "Karta statystyczna zawarcia małżeństwa". Dane według miejsca zameldowania męża przed ślubem, w przypadku gdy mąż przed ślubem mieszkał za granicą przyjmuje się miejsce zameldowania żony przed ślubem.</t>
+    <t>Małżeństwa na 1000 ludności</t>
+  </si>
+  <si>
+    <t>Dane dotyczące "małżeństw zawartych w ciągu roku na 1000 ludności" opracowane są według miejsca zameldowania męża przed ślubem, w przypadku gdy mąż przed ślubem mieszkał za granicą przyjmuje się miejsce zameldowania żony przed ślubem. Wskaźniki odnoszące się do liczby i struktury ludności (płeć, grupy wieku) od 2010 roku zostały przeliczone zgodnie z bilansem przygotowanym w oparciu o wyniki NSP 2011.</t>
   </si>
   <si>
     <t>Data ostatniej aktualizacji:</t>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Powiat bolesławiecki</t>
-  </si>
-  <si>
-    <t>0201032</t>
-  </si>
-  <si>
-    <t>Gromadka (2)</t>
   </si>
   <si>
     <t>0202000</t>
@@ -2335,7 +2329,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -2401,7 +2397,7 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2493,7 +2489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C384"/>
+  <dimension ref="A1:C383"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2532,7 +2528,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4">
-        <v>419</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="5">
@@ -2543,7 +2539,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="4">
-        <v>13</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="6">
@@ -2554,7 +2550,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="4">
-        <v>392</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="7">
@@ -2565,7 +2561,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="4">
-        <v>402</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -2576,7 +2572,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="4">
-        <v>176</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="9">
@@ -2587,7 +2583,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="4">
-        <v>221</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="10">
@@ -2598,7 +2594,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="4">
-        <v>230</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="11">
@@ -2609,7 +2605,7 @@
         <v>35</v>
       </c>
       <c r="C11" s="4">
-        <v>209</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="12">
@@ -2620,7 +2616,7 @@
         <v>37</v>
       </c>
       <c r="C12" s="4">
-        <v>718</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="13">
@@ -2631,7 +2627,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="4">
-        <v>245</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="14">
@@ -2642,7 +2638,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="4">
-        <v>249</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="15">
@@ -2653,7 +2649,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="4">
-        <v>561</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -2664,7 +2660,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="4">
-        <v>232</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="17">
@@ -2675,7 +2671,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="4">
-        <v>200</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -2686,7 +2682,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="4">
-        <v>533</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="19">
@@ -2697,7 +2693,7 @@
         <v>51</v>
       </c>
       <c r="C19" s="4">
-        <v>349</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="20">
@@ -2708,7 +2704,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="4">
-        <v>343</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="21">
@@ -2719,7 +2715,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="4">
-        <v>203</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="22">
@@ -2730,7 +2726,7 @@
         <v>57</v>
       </c>
       <c r="C22" s="4">
-        <v>258</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="23">
@@ -2741,7 +2737,7 @@
         <v>59</v>
       </c>
       <c r="C23" s="4">
-        <v>706</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="24">
@@ -2752,7 +2748,7 @@
         <v>61</v>
       </c>
       <c r="C24" s="4">
-        <v>385</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="25">
@@ -2763,7 +2759,7 @@
         <v>63</v>
       </c>
       <c r="C25" s="4">
-        <v>222</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="26">
@@ -2774,7 +2770,7 @@
         <v>65</v>
       </c>
       <c r="C26" s="4">
-        <v>261</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="27">
@@ -2785,7 +2781,7 @@
         <v>67</v>
       </c>
       <c r="C27" s="4">
-        <v>757</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="28">
@@ -2796,7 +2792,7 @@
         <v>69</v>
       </c>
       <c r="C28" s="4">
-        <v>290</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="29">
@@ -2807,7 +2803,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="4">
-        <v>410</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="30">
@@ -2818,7 +2814,7 @@
         <v>73</v>
       </c>
       <c r="C30" s="4">
-        <v>184</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="31">
@@ -2829,7 +2825,7 @@
         <v>75</v>
       </c>
       <c r="C31" s="4">
-        <v>377</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="32">
@@ -2840,7 +2836,7 @@
         <v>77</v>
       </c>
       <c r="C32" s="4">
-        <v>457</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="33">
@@ -2851,7 +2847,7 @@
         <v>79</v>
       </c>
       <c r="C33" s="4">
-        <v>3692</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="34">
@@ -2862,7 +2858,7 @@
         <v>81</v>
       </c>
       <c r="C34" s="4">
-        <v>459</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="35">
@@ -2873,7 +2869,7 @@
         <v>83</v>
       </c>
       <c r="C35" s="4">
-        <v>302</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="36">
@@ -2884,7 +2880,7 @@
         <v>85</v>
       </c>
       <c r="C36" s="4">
-        <v>453</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="37">
@@ -2895,7 +2891,7 @@
         <v>87</v>
       </c>
       <c r="C37" s="4">
-        <v>591</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="38">
@@ -2906,7 +2902,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="4">
-        <v>267</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="39">
@@ -2917,7 +2913,7 @@
         <v>91</v>
       </c>
       <c r="C39" s="4">
-        <v>209</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="40">
@@ -2928,7 +2924,7 @@
         <v>93</v>
       </c>
       <c r="C40" s="4">
-        <v>211</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="41">
@@ -2939,7 +2935,7 @@
         <v>95</v>
       </c>
       <c r="C41" s="4">
-        <v>782</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="42">
@@ -2950,7 +2946,7 @@
         <v>97</v>
       </c>
       <c r="C42" s="4">
-        <v>299</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="43">
@@ -2961,7 +2957,7 @@
         <v>99</v>
       </c>
       <c r="C43" s="4">
-        <v>251</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="44">
@@ -2972,7 +2968,7 @@
         <v>101</v>
       </c>
       <c r="C44" s="4">
-        <v>411</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -2983,7 +2979,7 @@
         <v>103</v>
       </c>
       <c r="C45" s="4">
-        <v>205</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="46">
@@ -2994,7 +2990,7 @@
         <v>105</v>
       </c>
       <c r="C46" s="4">
-        <v>240</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="47">
@@ -3005,7 +3001,7 @@
         <v>107</v>
       </c>
       <c r="C47" s="4">
-        <v>204</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="48">
@@ -3016,7 +3012,7 @@
         <v>109</v>
       </c>
       <c r="C48" s="4">
-        <v>461</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="49">
@@ -3027,7 +3023,7 @@
         <v>111</v>
       </c>
       <c r="C49" s="4">
-        <v>509</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="50">
@@ -3038,7 +3034,7 @@
         <v>113</v>
       </c>
       <c r="C50" s="4">
-        <v>284</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -3049,7 +3045,7 @@
         <v>115</v>
       </c>
       <c r="C51" s="4">
-        <v>174</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="52">
@@ -3060,7 +3056,7 @@
         <v>117</v>
       </c>
       <c r="C52" s="4">
-        <v>401</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -3071,7 +3067,7 @@
         <v>119</v>
       </c>
       <c r="C53" s="4">
-        <v>352</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="54">
@@ -3082,7 +3078,7 @@
         <v>121</v>
       </c>
       <c r="C54" s="4">
-        <v>1855</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="55">
@@ -3093,7 +3089,7 @@
         <v>123</v>
       </c>
       <c r="C55" s="4">
-        <v>465</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="56">
@@ -3104,7 +3100,7 @@
         <v>125</v>
       </c>
       <c r="C56" s="4">
-        <v>989</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
@@ -3115,7 +3111,7 @@
         <v>127</v>
       </c>
       <c r="C57" s="4">
-        <v>449</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="58">
@@ -3126,7 +3122,7 @@
         <v>129</v>
       </c>
       <c r="C58" s="4">
-        <v>542</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="59">
@@ -3137,7 +3133,7 @@
         <v>131</v>
       </c>
       <c r="C59" s="4">
-        <v>540</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -3148,7 +3144,7 @@
         <v>133</v>
       </c>
       <c r="C60" s="4">
-        <v>391</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="61">
@@ -3159,7 +3155,7 @@
         <v>135</v>
       </c>
       <c r="C61" s="4">
-        <v>313</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="62">
@@ -3170,7 +3166,7 @@
         <v>137</v>
       </c>
       <c r="C62" s="4">
-        <v>247</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="63">
@@ -3181,7 +3177,7 @@
         <v>139</v>
       </c>
       <c r="C63" s="4">
-        <v>294</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="64">
@@ -3192,7 +3188,7 @@
         <v>141</v>
       </c>
       <c r="C64" s="4">
-        <v>436</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="65">
@@ -3203,7 +3199,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="4">
-        <v>429</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="66">
@@ -3214,7 +3210,7 @@
         <v>145</v>
       </c>
       <c r="C66" s="4">
-        <v>724</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="67">
@@ -3225,7 +3221,7 @@
         <v>147</v>
       </c>
       <c r="C67" s="4">
-        <v>296</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="68">
@@ -3236,7 +3232,7 @@
         <v>149</v>
       </c>
       <c r="C68" s="4">
-        <v>620</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="69">
@@ -3247,7 +3243,7 @@
         <v>151</v>
       </c>
       <c r="C69" s="4">
-        <v>293</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="70">
@@ -3258,7 +3254,7 @@
         <v>153</v>
       </c>
       <c r="C70" s="4">
-        <v>195</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="71">
@@ -3269,7 +3265,7 @@
         <v>155</v>
       </c>
       <c r="C71" s="4">
-        <v>540</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="72">
@@ -3280,7 +3276,7 @@
         <v>157</v>
       </c>
       <c r="C72" s="4">
-        <v>302</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="73">
@@ -3288,21 +3284,21 @@
         <v>158</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="C73" s="4">
-        <v>289</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="C74" s="4">
-        <v>319</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="75">
@@ -3313,7 +3309,7 @@
         <v>162</v>
       </c>
       <c r="C75" s="4">
-        <v>397</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="76">
@@ -3324,7 +3320,7 @@
         <v>164</v>
       </c>
       <c r="C76" s="4">
-        <v>169</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="77">
@@ -3335,7 +3331,7 @@
         <v>166</v>
       </c>
       <c r="C77" s="4">
-        <v>561</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="78">
@@ -3346,7 +3342,7 @@
         <v>168</v>
       </c>
       <c r="C78" s="4">
-        <v>294</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="79">
@@ -3357,7 +3353,7 @@
         <v>170</v>
       </c>
       <c r="C79" s="4">
-        <v>289</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -3368,7 +3364,7 @@
         <v>172</v>
       </c>
       <c r="C80" s="4">
-        <v>1709</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -3379,7 +3375,7 @@
         <v>174</v>
       </c>
       <c r="C81" s="4">
-        <v>320</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="82">
@@ -3390,7 +3386,7 @@
         <v>176</v>
       </c>
       <c r="C82" s="4">
-        <v>309</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="83">
@@ -3401,7 +3397,7 @@
         <v>178</v>
       </c>
       <c r="C83" s="4">
-        <v>262</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -3412,7 +3408,7 @@
         <v>180</v>
       </c>
       <c r="C84" s="4">
-        <v>291</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="85">
@@ -3423,7 +3419,7 @@
         <v>182</v>
       </c>
       <c r="C85" s="4">
-        <v>409</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="86">
@@ -3434,7 +3430,7 @@
         <v>184</v>
       </c>
       <c r="C86" s="4">
-        <v>232</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="87">
@@ -3445,7 +3441,7 @@
         <v>186</v>
       </c>
       <c r="C87" s="4">
-        <v>220</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="88">
@@ -3456,7 +3452,7 @@
         <v>188</v>
       </c>
       <c r="C88" s="4">
-        <v>162</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="89">
@@ -3467,7 +3463,7 @@
         <v>190</v>
       </c>
       <c r="C89" s="4">
-        <v>294</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="90">
@@ -3478,7 +3474,7 @@
         <v>192</v>
       </c>
       <c r="C90" s="4">
-        <v>350</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="91">
@@ -3489,7 +3485,7 @@
         <v>194</v>
       </c>
       <c r="C91" s="4">
-        <v>412</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="92">
@@ -3500,7 +3496,7 @@
         <v>196</v>
       </c>
       <c r="C92" s="4">
-        <v>473</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="93">
@@ -3511,7 +3507,7 @@
         <v>198</v>
       </c>
       <c r="C93" s="4">
-        <v>201</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="94">
@@ -3522,7 +3518,7 @@
         <v>200</v>
       </c>
       <c r="C94" s="4">
-        <v>694</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="95">
@@ -3533,7 +3529,7 @@
         <v>202</v>
       </c>
       <c r="C95" s="4">
-        <v>626</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -3544,7 +3540,7 @@
         <v>204</v>
       </c>
       <c r="C96" s="4">
-        <v>567</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="97">
@@ -3555,7 +3551,7 @@
         <v>206</v>
       </c>
       <c r="C97" s="4">
-        <v>450</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="98">
@@ -3566,7 +3562,7 @@
         <v>208</v>
       </c>
       <c r="C98" s="4">
-        <v>221</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="99">
@@ -3577,7 +3573,7 @@
         <v>210</v>
       </c>
       <c r="C99" s="4">
-        <v>237</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="100">
@@ -3588,7 +3584,7 @@
         <v>212</v>
       </c>
       <c r="C100" s="4">
-        <v>400</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="101">
@@ -3599,7 +3595,7 @@
         <v>214</v>
       </c>
       <c r="C101" s="4">
-        <v>290</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102">
@@ -3610,7 +3606,7 @@
         <v>216</v>
       </c>
       <c r="C102" s="4">
-        <v>386</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="103">
@@ -3621,7 +3617,7 @@
         <v>218</v>
       </c>
       <c r="C103" s="4">
-        <v>505</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="104">
@@ -3632,7 +3628,7 @@
         <v>220</v>
       </c>
       <c r="C104" s="4">
-        <v>245</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
@@ -3643,7 +3639,7 @@
         <v>222</v>
       </c>
       <c r="C105" s="4">
-        <v>454</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="106">
@@ -3654,7 +3650,7 @@
         <v>224</v>
       </c>
       <c r="C106" s="4">
-        <v>218</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="107">
@@ -3665,7 +3661,7 @@
         <v>226</v>
       </c>
       <c r="C107" s="4">
-        <v>526</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="108">
@@ -3676,7 +3672,7 @@
         <v>228</v>
       </c>
       <c r="C108" s="4">
-        <v>247</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="109">
@@ -3687,7 +3683,7 @@
         <v>230</v>
       </c>
       <c r="C109" s="4">
-        <v>603</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -3695,21 +3691,21 @@
         <v>231</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="C110" s="4">
-        <v>190</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B111" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>162</v>
-      </c>
       <c r="C111" s="4">
-        <v>533</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112">
@@ -3720,7 +3716,7 @@
         <v>235</v>
       </c>
       <c r="C112" s="4">
-        <v>382</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="113">
@@ -3731,7 +3727,7 @@
         <v>237</v>
       </c>
       <c r="C113" s="4">
-        <v>179</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="114">
@@ -3742,7 +3738,7 @@
         <v>239</v>
       </c>
       <c r="C114" s="4">
-        <v>315</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="115">
@@ -3753,7 +3749,7 @@
         <v>241</v>
       </c>
       <c r="C115" s="4">
-        <v>710</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="116">
@@ -3764,7 +3760,7 @@
         <v>243</v>
       </c>
       <c r="C116" s="4">
-        <v>136</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="117">
@@ -3775,7 +3771,7 @@
         <v>245</v>
       </c>
       <c r="C117" s="4">
-        <v>3209</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="118">
@@ -3786,7 +3782,7 @@
         <v>247</v>
       </c>
       <c r="C118" s="4">
-        <v>310</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119">
@@ -3797,7 +3793,7 @@
         <v>249</v>
       </c>
       <c r="C119" s="4">
-        <v>242</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="120">
@@ -3808,7 +3804,7 @@
         <v>251</v>
       </c>
       <c r="C120" s="4">
-        <v>588</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="121">
@@ -3819,7 +3815,7 @@
         <v>253</v>
       </c>
       <c r="C121" s="4">
-        <v>501</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="122">
@@ -3830,7 +3826,7 @@
         <v>255</v>
       </c>
       <c r="C122" s="4">
-        <v>612</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="123">
@@ -3841,7 +3837,7 @@
         <v>257</v>
       </c>
       <c r="C123" s="4">
-        <v>310</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="124">
@@ -3852,7 +3848,7 @@
         <v>259</v>
       </c>
       <c r="C124" s="4">
-        <v>570</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="125">
@@ -3863,7 +3859,7 @@
         <v>261</v>
       </c>
       <c r="C125" s="4">
-        <v>1318</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="126">
@@ -3874,7 +3870,7 @@
         <v>263</v>
       </c>
       <c r="C126" s="4">
-        <v>840</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="127">
@@ -3885,7 +3881,7 @@
         <v>265</v>
       </c>
       <c r="C127" s="4">
-        <v>239</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="128">
@@ -3896,7 +3892,7 @@
         <v>267</v>
       </c>
       <c r="C128" s="4">
-        <v>776</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="129">
@@ -3907,7 +3903,7 @@
         <v>269</v>
       </c>
       <c r="C129" s="4">
-        <v>1338</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130">
@@ -3918,7 +3914,7 @@
         <v>271</v>
       </c>
       <c r="C130" s="4">
-        <v>962</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="131">
@@ -3929,7 +3925,7 @@
         <v>273</v>
       </c>
       <c r="C131" s="4">
-        <v>546</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -3940,7 +3936,7 @@
         <v>275</v>
       </c>
       <c r="C132" s="4">
-        <v>773</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="133">
@@ -3951,7 +3947,7 @@
         <v>277</v>
       </c>
       <c r="C133" s="4">
-        <v>230</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="134">
@@ -3962,7 +3958,7 @@
         <v>279</v>
       </c>
       <c r="C134" s="4">
-        <v>475</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="135">
@@ -3973,7 +3969,7 @@
         <v>281</v>
       </c>
       <c r="C135" s="4">
-        <v>1126</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="136">
@@ -3984,7 +3980,7 @@
         <v>283</v>
       </c>
       <c r="C136" s="4">
-        <v>315</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="137">
@@ -3995,7 +3991,7 @@
         <v>285</v>
       </c>
       <c r="C137" s="4">
-        <v>842</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="138">
@@ -4006,7 +4002,7 @@
         <v>287</v>
       </c>
       <c r="C138" s="4">
-        <v>650</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="139">
@@ -4017,7 +4013,7 @@
         <v>289</v>
       </c>
       <c r="C139" s="4">
-        <v>4498</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="140">
@@ -4028,7 +4024,7 @@
         <v>291</v>
       </c>
       <c r="C140" s="4">
-        <v>462</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="141">
@@ -4039,7 +4035,7 @@
         <v>293</v>
       </c>
       <c r="C141" s="4">
-        <v>479</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="142">
@@ -4050,7 +4046,7 @@
         <v>295</v>
       </c>
       <c r="C142" s="4">
-        <v>188</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="143">
@@ -4061,7 +4057,7 @@
         <v>297</v>
       </c>
       <c r="C143" s="4">
-        <v>474</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="144">
@@ -4072,7 +4068,7 @@
         <v>299</v>
       </c>
       <c r="C144" s="4">
-        <v>621</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="145">
@@ -4083,7 +4079,7 @@
         <v>301</v>
       </c>
       <c r="C145" s="4">
-        <v>211</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="146">
@@ -4094,7 +4090,7 @@
         <v>303</v>
       </c>
       <c r="C146" s="4">
-        <v>416</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="147">
@@ -4105,7 +4101,7 @@
         <v>305</v>
       </c>
       <c r="C147" s="4">
-        <v>483</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="148">
@@ -4116,7 +4112,7 @@
         <v>307</v>
       </c>
       <c r="C148" s="4">
-        <v>327</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="149">
@@ -4127,7 +4123,7 @@
         <v>309</v>
       </c>
       <c r="C149" s="4">
-        <v>551</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150">
@@ -4138,7 +4134,7 @@
         <v>311</v>
       </c>
       <c r="C150" s="4">
-        <v>173</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="151">
@@ -4149,7 +4145,7 @@
         <v>313</v>
       </c>
       <c r="C151" s="4">
-        <v>147</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="152">
@@ -4160,7 +4156,7 @@
         <v>315</v>
       </c>
       <c r="C152" s="4">
-        <v>240</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="153">
@@ -4171,7 +4167,7 @@
         <v>317</v>
       </c>
       <c r="C153" s="4">
-        <v>715</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="154">
@@ -4182,7 +4178,7 @@
         <v>319</v>
       </c>
       <c r="C154" s="4">
-        <v>380</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="155">
@@ -4193,7 +4189,7 @@
         <v>321</v>
       </c>
       <c r="C155" s="4">
-        <v>368</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="156">
@@ -4204,7 +4200,7 @@
         <v>323</v>
       </c>
       <c r="C156" s="4">
-        <v>493</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="157">
@@ -4215,7 +4211,7 @@
         <v>325</v>
       </c>
       <c r="C157" s="4">
-        <v>378</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="158">
@@ -4226,7 +4222,7 @@
         <v>327</v>
       </c>
       <c r="C158" s="4">
-        <v>540</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="159">
@@ -4237,7 +4233,7 @@
         <v>329</v>
       </c>
       <c r="C159" s="4">
-        <v>818</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="160">
@@ -4248,7 +4244,7 @@
         <v>331</v>
       </c>
       <c r="C160" s="4">
-        <v>521</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="161">
@@ -4259,7 +4255,7 @@
         <v>333</v>
       </c>
       <c r="C161" s="4">
-        <v>427</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="162">
@@ -4270,7 +4266,7 @@
         <v>335</v>
       </c>
       <c r="C162" s="4">
-        <v>789</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163">
@@ -4281,7 +4277,7 @@
         <v>337</v>
       </c>
       <c r="C163" s="4">
-        <v>265</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="164">
@@ -4292,7 +4288,7 @@
         <v>339</v>
       </c>
       <c r="C164" s="4">
-        <v>236</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="165">
@@ -4303,7 +4299,7 @@
         <v>341</v>
       </c>
       <c r="C165" s="4">
-        <v>289</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="166">
@@ -4314,7 +4310,7 @@
         <v>343</v>
       </c>
       <c r="C166" s="4">
-        <v>835</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="167">
@@ -4325,7 +4321,7 @@
         <v>345</v>
       </c>
       <c r="C167" s="4">
-        <v>467</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="168">
@@ -4336,7 +4332,7 @@
         <v>347</v>
       </c>
       <c r="C168" s="4">
-        <v>268</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="169">
@@ -4347,7 +4343,7 @@
         <v>349</v>
       </c>
       <c r="C169" s="4">
-        <v>408</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="170">
@@ -4358,7 +4354,7 @@
         <v>351</v>
       </c>
       <c r="C170" s="4">
-        <v>285</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="171">
@@ -4369,7 +4365,7 @@
         <v>353</v>
       </c>
       <c r="C171" s="4">
-        <v>187</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="172">
@@ -4380,7 +4376,7 @@
         <v>355</v>
       </c>
       <c r="C172" s="4">
-        <v>573</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="173">
@@ -4391,7 +4387,7 @@
         <v>357</v>
       </c>
       <c r="C173" s="4">
-        <v>365</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="174">
@@ -4402,7 +4398,7 @@
         <v>359</v>
       </c>
       <c r="C174" s="4">
-        <v>1284</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="175">
@@ -4413,7 +4409,7 @@
         <v>361</v>
       </c>
       <c r="C175" s="4">
-        <v>386</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="176">
@@ -4424,7 +4420,7 @@
         <v>363</v>
       </c>
       <c r="C176" s="4">
-        <v>197</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177">
@@ -4435,7 +4431,7 @@
         <v>365</v>
       </c>
       <c r="C177" s="4">
-        <v>197</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="178">
@@ -4446,7 +4442,7 @@
         <v>367</v>
       </c>
       <c r="C178" s="4">
-        <v>361</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="179">
@@ -4457,7 +4453,7 @@
         <v>369</v>
       </c>
       <c r="C179" s="4">
-        <v>265</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="180">
@@ -4468,7 +4464,7 @@
         <v>371</v>
       </c>
       <c r="C180" s="4">
-        <v>534</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="181">
@@ -4479,7 +4475,7 @@
         <v>373</v>
       </c>
       <c r="C181" s="4">
-        <v>1007</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182">
@@ -4490,7 +4486,7 @@
         <v>375</v>
       </c>
       <c r="C182" s="4">
-        <v>387</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="183">
@@ -4498,21 +4494,21 @@
         <v>376</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="C183" s="4">
-        <v>9164</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B184" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="B184" s="0" t="s">
-        <v>253</v>
-      </c>
       <c r="C184" s="4">
-        <v>402</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="185">
@@ -4523,7 +4519,7 @@
         <v>380</v>
       </c>
       <c r="C185" s="4">
-        <v>202</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="186">
@@ -4534,7 +4530,7 @@
         <v>382</v>
       </c>
       <c r="C186" s="4">
-        <v>414</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="187">
@@ -4545,7 +4541,7 @@
         <v>384</v>
       </c>
       <c r="C187" s="4">
-        <v>324</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="188">
@@ -4556,7 +4552,7 @@
         <v>386</v>
       </c>
       <c r="C188" s="4">
-        <v>293</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="189">
@@ -4567,7 +4563,7 @@
         <v>388</v>
       </c>
       <c r="C189" s="4">
-        <v>194</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190">
@@ -4578,7 +4574,7 @@
         <v>390</v>
       </c>
       <c r="C190" s="4">
-        <v>687</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="191">
@@ -4586,21 +4582,21 @@
         <v>391</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>392</v>
+        <v>149</v>
       </c>
       <c r="C191" s="4">
-        <v>314</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B192" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="B192" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="C192" s="4">
-        <v>573</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193">
@@ -4611,7 +4607,7 @@
         <v>395</v>
       </c>
       <c r="C193" s="4">
-        <v>280</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="194">
@@ -4622,7 +4618,7 @@
         <v>397</v>
       </c>
       <c r="C194" s="4">
-        <v>406</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="195">
@@ -4633,7 +4629,7 @@
         <v>399</v>
       </c>
       <c r="C195" s="4">
-        <v>621</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="196">
@@ -4644,7 +4640,7 @@
         <v>401</v>
       </c>
       <c r="C196" s="4">
-        <v>112</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="197">
@@ -4655,7 +4651,7 @@
         <v>403</v>
       </c>
       <c r="C197" s="4">
-        <v>381</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="198">
@@ -4666,7 +4662,7 @@
         <v>405</v>
       </c>
       <c r="C198" s="4">
-        <v>738</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199">
@@ -4677,7 +4673,7 @@
         <v>407</v>
       </c>
       <c r="C199" s="4">
-        <v>604</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200">
@@ -4688,7 +4684,7 @@
         <v>409</v>
       </c>
       <c r="C200" s="4">
-        <v>568</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="201">
@@ -4696,21 +4692,21 @@
         <v>410</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>411</v>
+        <v>176</v>
       </c>
       <c r="C201" s="4">
-        <v>328</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B202" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="B202" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="C202" s="4">
-        <v>535</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203">
@@ -4721,7 +4717,7 @@
         <v>414</v>
       </c>
       <c r="C203" s="4">
-        <v>346</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="204">
@@ -4732,7 +4728,7 @@
         <v>416</v>
       </c>
       <c r="C204" s="4">
-        <v>274</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="205">
@@ -4743,7 +4739,7 @@
         <v>418</v>
       </c>
       <c r="C205" s="4">
-        <v>414</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="206">
@@ -4754,7 +4750,7 @@
         <v>420</v>
       </c>
       <c r="C206" s="4">
-        <v>730</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="207">
@@ -4765,7 +4761,7 @@
         <v>422</v>
       </c>
       <c r="C207" s="4">
-        <v>374</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="208">
@@ -4776,7 +4772,7 @@
         <v>424</v>
       </c>
       <c r="C208" s="4">
-        <v>378</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="209">
@@ -4787,7 +4783,7 @@
         <v>426</v>
       </c>
       <c r="C209" s="4">
-        <v>455</v>
+        <v>6</v>
       </c>
     </row>
     <row r="210">
@@ -4798,7 +4794,7 @@
         <v>428</v>
       </c>
       <c r="C210" s="4">
-        <v>447</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="211">
@@ -4809,7 +4805,7 @@
         <v>430</v>
       </c>
       <c r="C211" s="4">
-        <v>867</v>
+        <v>5</v>
       </c>
     </row>
     <row r="212">
@@ -4820,7 +4816,7 @@
         <v>432</v>
       </c>
       <c r="C212" s="4">
-        <v>477</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213">
@@ -4831,7 +4827,7 @@
         <v>434</v>
       </c>
       <c r="C213" s="4">
-        <v>538</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="214">
@@ -4842,7 +4838,7 @@
         <v>436</v>
       </c>
       <c r="C214" s="4">
-        <v>305</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215">
@@ -4853,7 +4849,7 @@
         <v>438</v>
       </c>
       <c r="C215" s="4">
-        <v>266</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="216">
@@ -4864,7 +4860,7 @@
         <v>440</v>
       </c>
       <c r="C216" s="4">
-        <v>121</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="217">
@@ -4875,7 +4871,7 @@
         <v>442</v>
       </c>
       <c r="C217" s="4">
-        <v>212</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="218">
@@ -4886,7 +4882,7 @@
         <v>444</v>
       </c>
       <c r="C218" s="4">
-        <v>251</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="219">
@@ -4897,7 +4893,7 @@
         <v>446</v>
       </c>
       <c r="C219" s="4">
-        <v>928</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="220">
@@ -4908,7 +4904,7 @@
         <v>448</v>
       </c>
       <c r="C220" s="4">
-        <v>225</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="221">
@@ -4919,7 +4915,7 @@
         <v>450</v>
       </c>
       <c r="C221" s="4">
-        <v>299</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222">
@@ -4930,7 +4926,7 @@
         <v>452</v>
       </c>
       <c r="C222" s="4">
-        <v>732</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="223">
@@ -4941,7 +4937,7 @@
         <v>454</v>
       </c>
       <c r="C223" s="4">
-        <v>301</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="224">
@@ -4952,7 +4948,7 @@
         <v>456</v>
       </c>
       <c r="C224" s="4">
-        <v>205</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="225">
@@ -4963,7 +4959,7 @@
         <v>458</v>
       </c>
       <c r="C225" s="4">
-        <v>206</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="226">
@@ -4974,7 +4970,7 @@
         <v>460</v>
       </c>
       <c r="C226" s="4">
-        <v>182</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="227">
@@ -4985,7 +4981,7 @@
         <v>462</v>
       </c>
       <c r="C227" s="4">
-        <v>297</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="228">
@@ -4996,7 +4992,7 @@
         <v>464</v>
       </c>
       <c r="C228" s="4">
-        <v>220</v>
+        <v>5</v>
       </c>
     </row>
     <row r="229">
@@ -5007,7 +5003,7 @@
         <v>466</v>
       </c>
       <c r="C229" s="4">
-        <v>100</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="230">
@@ -5018,7 +5014,7 @@
         <v>468</v>
       </c>
       <c r="C230" s="4">
-        <v>218</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="231">
@@ -5029,7 +5025,7 @@
         <v>470</v>
       </c>
       <c r="C231" s="4">
-        <v>322</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="232">
@@ -5040,7 +5036,7 @@
         <v>472</v>
       </c>
       <c r="C232" s="4">
-        <v>187</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="233">
@@ -5051,7 +5047,7 @@
         <v>474</v>
       </c>
       <c r="C233" s="4">
-        <v>292</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="234">
@@ -5062,7 +5058,7 @@
         <v>476</v>
       </c>
       <c r="C234" s="4">
-        <v>239</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="235">
@@ -5073,7 +5069,7 @@
         <v>478</v>
       </c>
       <c r="C235" s="4">
-        <v>1470</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="236">
@@ -5084,7 +5080,7 @@
         <v>480</v>
       </c>
       <c r="C236" s="4">
-        <v>341</v>
+        <v>5</v>
       </c>
     </row>
     <row r="237">
@@ -5095,7 +5091,7 @@
         <v>482</v>
       </c>
       <c r="C237" s="4">
-        <v>345</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="238">
@@ -5106,7 +5102,7 @@
         <v>484</v>
       </c>
       <c r="C238" s="4">
-        <v>457</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="239">
@@ -5117,7 +5113,7 @@
         <v>486</v>
       </c>
       <c r="C239" s="4">
-        <v>547</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="240">
@@ -5128,7 +5124,7 @@
         <v>488</v>
       </c>
       <c r="C240" s="4">
-        <v>300</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="241">
@@ -5139,7 +5135,7 @@
         <v>490</v>
       </c>
       <c r="C241" s="4">
-        <v>623</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="242">
@@ -5150,7 +5146,7 @@
         <v>492</v>
       </c>
       <c r="C242" s="4">
-        <v>827</v>
+        <v>5</v>
       </c>
     </row>
     <row r="243">
@@ -5161,7 +5157,7 @@
         <v>494</v>
       </c>
       <c r="C243" s="4">
-        <v>365</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="244">
@@ -5172,7 +5168,7 @@
         <v>496</v>
       </c>
       <c r="C244" s="4">
-        <v>407</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="245">
@@ -5183,7 +5179,7 @@
         <v>498</v>
       </c>
       <c r="C245" s="4">
-        <v>328</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="246">
@@ -5191,21 +5187,21 @@
         <v>499</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>500</v>
+        <v>319</v>
       </c>
       <c r="C246" s="4">
-        <v>286</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B247" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="B247" s="0" t="s">
-        <v>321</v>
-      </c>
       <c r="C247" s="4">
-        <v>169</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="248">
@@ -5216,7 +5212,7 @@
         <v>503</v>
       </c>
       <c r="C248" s="4">
-        <v>459</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="249">
@@ -5227,7 +5223,7 @@
         <v>505</v>
       </c>
       <c r="C249" s="4">
-        <v>443</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="250">
@@ -5238,7 +5234,7 @@
         <v>507</v>
       </c>
       <c r="C250" s="4">
-        <v>684</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="251">
@@ -5249,7 +5245,7 @@
         <v>509</v>
       </c>
       <c r="C251" s="4">
-        <v>561</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="252">
@@ -5260,7 +5256,7 @@
         <v>511</v>
       </c>
       <c r="C252" s="4">
-        <v>1254</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="253">
@@ -5271,7 +5267,7 @@
         <v>513</v>
       </c>
       <c r="C253" s="4">
-        <v>185</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="254">
@@ -5282,7 +5278,7 @@
         <v>515</v>
       </c>
       <c r="C254" s="4">
-        <v>2669</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="255">
@@ -5293,7 +5289,7 @@
         <v>517</v>
       </c>
       <c r="C255" s="4">
-        <v>1326</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="256">
@@ -5304,7 +5300,7 @@
         <v>519</v>
       </c>
       <c r="C256" s="4">
-        <v>415</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="257">
@@ -5315,7 +5311,7 @@
         <v>521</v>
       </c>
       <c r="C257" s="4">
-        <v>168</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="258">
@@ -5323,21 +5319,21 @@
         <v>522</v>
       </c>
       <c r="B258" s="0" t="s">
-        <v>523</v>
+        <v>452</v>
       </c>
       <c r="C258" s="4">
-        <v>624</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="B259" s="0" t="s">
         <v>524</v>
       </c>
-      <c r="B259" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="C259" s="4">
-        <v>857</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260">
@@ -5348,7 +5344,7 @@
         <v>526</v>
       </c>
       <c r="C260" s="4">
-        <v>894</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="261">
@@ -5359,7 +5355,7 @@
         <v>528</v>
       </c>
       <c r="C261" s="4">
-        <v>621</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="262">
@@ -5370,7 +5366,7 @@
         <v>530</v>
       </c>
       <c r="C262" s="4">
-        <v>609</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="263">
@@ -5381,7 +5377,7 @@
         <v>532</v>
       </c>
       <c r="C263" s="4">
-        <v>457</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="264">
@@ -5392,7 +5388,7 @@
         <v>534</v>
       </c>
       <c r="C264" s="4">
-        <v>368</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="265">
@@ -5403,7 +5399,7 @@
         <v>536</v>
       </c>
       <c r="C265" s="4">
-        <v>509</v>
+        <v>5</v>
       </c>
     </row>
     <row r="266">
@@ -5414,7 +5410,7 @@
         <v>538</v>
       </c>
       <c r="C266" s="4">
-        <v>354</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="267">
@@ -5425,7 +5421,7 @@
         <v>540</v>
       </c>
       <c r="C267" s="4">
-        <v>596</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="268">
@@ -5436,7 +5432,7 @@
         <v>542</v>
       </c>
       <c r="C268" s="4">
-        <v>522</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="269">
@@ -5447,7 +5443,7 @@
         <v>544</v>
       </c>
       <c r="C269" s="4">
-        <v>377</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="270">
@@ -5458,7 +5454,7 @@
         <v>546</v>
       </c>
       <c r="C270" s="4">
-        <v>657</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="271">
@@ -5469,7 +5465,7 @@
         <v>548</v>
       </c>
       <c r="C271" s="4">
-        <v>313</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="272">
@@ -5480,7 +5476,7 @@
         <v>550</v>
       </c>
       <c r="C272" s="4">
-        <v>769</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="273">
@@ -5491,7 +5487,7 @@
         <v>552</v>
       </c>
       <c r="C273" s="4">
-        <v>516</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="274">
@@ -5502,7 +5498,7 @@
         <v>554</v>
       </c>
       <c r="C274" s="4">
-        <v>753</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="275">
@@ -5513,7 +5509,7 @@
         <v>556</v>
       </c>
       <c r="C275" s="4">
-        <v>842</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="276">
@@ -5524,7 +5520,7 @@
         <v>558</v>
       </c>
       <c r="C276" s="4">
-        <v>821</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="277">
@@ -5535,7 +5531,7 @@
         <v>560</v>
       </c>
       <c r="C277" s="4">
-        <v>514</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="278">
@@ -5546,7 +5542,7 @@
         <v>562</v>
       </c>
       <c r="C278" s="4">
-        <v>990</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="279">
@@ -5557,7 +5553,7 @@
         <v>564</v>
       </c>
       <c r="C279" s="4">
-        <v>471</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="280">
@@ -5568,7 +5564,7 @@
         <v>566</v>
       </c>
       <c r="C280" s="4">
-        <v>925</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="281">
@@ -5579,7 +5575,7 @@
         <v>568</v>
       </c>
       <c r="C281" s="4">
-        <v>431</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="282">
@@ -5590,7 +5586,7 @@
         <v>570</v>
       </c>
       <c r="C282" s="4">
-        <v>447</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="283">
@@ -5601,7 +5597,7 @@
         <v>572</v>
       </c>
       <c r="C283" s="4">
-        <v>1552</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="284">
@@ -5612,7 +5608,7 @@
         <v>574</v>
       </c>
       <c r="C284" s="4">
-        <v>402</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285">
@@ -5623,7 +5619,7 @@
         <v>576</v>
       </c>
       <c r="C285" s="4">
-        <v>280</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="286">
@@ -5634,7 +5630,7 @@
         <v>578</v>
       </c>
       <c r="C286" s="4">
-        <v>720</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="287">
@@ -5645,7 +5641,7 @@
         <v>580</v>
       </c>
       <c r="C287" s="4">
-        <v>713</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="288">
@@ -5656,7 +5652,7 @@
         <v>582</v>
       </c>
       <c r="C288" s="4">
-        <v>378</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="289">
@@ -5667,7 +5663,7 @@
         <v>584</v>
       </c>
       <c r="C289" s="4">
-        <v>987</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="290">
@@ -5678,7 +5674,7 @@
         <v>586</v>
       </c>
       <c r="C290" s="4">
-        <v>256</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="291">
@@ -5689,7 +5685,7 @@
         <v>588</v>
       </c>
       <c r="C291" s="4">
-        <v>596</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="292">
@@ -5700,7 +5696,7 @@
         <v>590</v>
       </c>
       <c r="C292" s="4">
-        <v>800</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="293">
@@ -5711,7 +5707,7 @@
         <v>592</v>
       </c>
       <c r="C293" s="4">
-        <v>321</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="294">
@@ -5722,7 +5718,7 @@
         <v>594</v>
       </c>
       <c r="C294" s="4">
-        <v>335</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="295">
@@ -5733,7 +5729,7 @@
         <v>596</v>
       </c>
       <c r="C295" s="4">
-        <v>409</v>
+        <v>4</v>
       </c>
     </row>
     <row r="296">
@@ -5744,7 +5740,7 @@
         <v>598</v>
       </c>
       <c r="C296" s="4">
-        <v>137</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="297">
@@ -5755,7 +5751,7 @@
         <v>600</v>
       </c>
       <c r="C297" s="4">
-        <v>1080</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="298">
@@ -5766,7 +5762,7 @@
         <v>602</v>
       </c>
       <c r="C298" s="4">
-        <v>370</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="299">
@@ -5777,7 +5773,7 @@
         <v>604</v>
       </c>
       <c r="C299" s="4">
-        <v>243</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="300">
@@ -5788,7 +5784,7 @@
         <v>606</v>
       </c>
       <c r="C300" s="4">
-        <v>467</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="301">
@@ -5799,7 +5795,7 @@
         <v>608</v>
       </c>
       <c r="C301" s="4">
-        <v>210</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="302">
@@ -5810,7 +5806,7 @@
         <v>610</v>
       </c>
       <c r="C302" s="4">
-        <v>377</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="303">
@@ -5821,7 +5817,7 @@
         <v>612</v>
       </c>
       <c r="C303" s="4">
-        <v>350</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="304">
@@ -5832,7 +5828,7 @@
         <v>614</v>
       </c>
       <c r="C304" s="4">
-        <v>375</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="305">
@@ -5843,7 +5839,7 @@
         <v>616</v>
       </c>
       <c r="C305" s="4">
-        <v>372</v>
+        <v>6</v>
       </c>
     </row>
     <row r="306">
@@ -5854,7 +5850,7 @@
         <v>618</v>
       </c>
       <c r="C306" s="4">
-        <v>274</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="307">
@@ -5865,7 +5861,7 @@
         <v>620</v>
       </c>
       <c r="C307" s="4">
-        <v>903</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="308">
@@ -5876,7 +5872,7 @@
         <v>622</v>
       </c>
       <c r="C308" s="4">
-        <v>277</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="309">
@@ -5887,7 +5883,7 @@
         <v>624</v>
       </c>
       <c r="C309" s="4">
-        <v>186</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="310">
@@ -5898,7 +5894,7 @@
         <v>626</v>
       </c>
       <c r="C310" s="4">
-        <v>335</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="311">
@@ -5909,7 +5905,7 @@
         <v>628</v>
       </c>
       <c r="C311" s="4">
-        <v>251</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="312">
@@ -5920,7 +5916,7 @@
         <v>630</v>
       </c>
       <c r="C312" s="4">
-        <v>412</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="313">
@@ -5931,7 +5927,7 @@
         <v>632</v>
       </c>
       <c r="C313" s="4">
-        <v>262</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314">
@@ -5942,7 +5938,7 @@
         <v>634</v>
       </c>
       <c r="C314" s="4">
-        <v>468</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="315">
@@ -5953,7 +5949,7 @@
         <v>636</v>
       </c>
       <c r="C315" s="4">
-        <v>279</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="316">
@@ -5964,7 +5960,7 @@
         <v>638</v>
       </c>
       <c r="C316" s="4">
-        <v>179</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="317">
@@ -5975,7 +5971,7 @@
         <v>640</v>
       </c>
       <c r="C317" s="4">
-        <v>246</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="318">
@@ -5986,7 +5982,7 @@
         <v>642</v>
       </c>
       <c r="C318" s="4">
-        <v>140</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="319">
@@ -5997,7 +5993,7 @@
         <v>644</v>
       </c>
       <c r="C319" s="4">
-        <v>229</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="320">
@@ -6008,7 +6004,7 @@
         <v>646</v>
       </c>
       <c r="C320" s="4">
-        <v>159</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="321">
@@ -6019,7 +6015,7 @@
         <v>648</v>
       </c>
       <c r="C321" s="4">
-        <v>608</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="322">
@@ -6030,7 +6026,7 @@
         <v>650</v>
       </c>
       <c r="C322" s="4">
-        <v>489</v>
+        <v>5</v>
       </c>
     </row>
     <row r="323">
@@ -6041,7 +6037,7 @@
         <v>652</v>
       </c>
       <c r="C323" s="4">
-        <v>286</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="324">
@@ -6052,7 +6048,7 @@
         <v>654</v>
       </c>
       <c r="C324" s="4">
-        <v>327</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="325">
@@ -6063,7 +6059,7 @@
         <v>656</v>
       </c>
       <c r="C325" s="4">
-        <v>155</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="326">
@@ -6074,7 +6070,7 @@
         <v>658</v>
       </c>
       <c r="C326" s="4">
-        <v>105</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="327">
@@ -6085,7 +6081,7 @@
         <v>660</v>
       </c>
       <c r="C327" s="4">
-        <v>573</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="328">
@@ -6096,7 +6092,7 @@
         <v>662</v>
       </c>
       <c r="C328" s="4">
-        <v>730</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="329">
@@ -6107,7 +6103,7 @@
         <v>664</v>
       </c>
       <c r="C329" s="4">
-        <v>228</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="330">
@@ -6118,7 +6114,7 @@
         <v>666</v>
       </c>
       <c r="C330" s="4">
-        <v>421</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="331">
@@ -6129,7 +6125,7 @@
         <v>668</v>
       </c>
       <c r="C331" s="4">
-        <v>751</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="332">
@@ -6137,21 +6133,21 @@
         <v>669</v>
       </c>
       <c r="B332" s="0" t="s">
-        <v>670</v>
+        <v>301</v>
       </c>
       <c r="C332" s="4">
-        <v>444</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="B333" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="B333" s="0" t="s">
-        <v>303</v>
-      </c>
       <c r="C333" s="4">
-        <v>282</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="334">
@@ -6162,7 +6158,7 @@
         <v>673</v>
       </c>
       <c r="C334" s="4">
-        <v>366</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="335">
@@ -6173,7 +6169,7 @@
         <v>675</v>
       </c>
       <c r="C335" s="4">
-        <v>424</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="336">
@@ -6184,7 +6180,7 @@
         <v>677</v>
       </c>
       <c r="C336" s="4">
-        <v>260</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="337">
@@ -6195,7 +6191,7 @@
         <v>679</v>
       </c>
       <c r="C337" s="4">
-        <v>448</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="338">
@@ -6206,7 +6202,7 @@
         <v>681</v>
       </c>
       <c r="C338" s="4">
-        <v>638</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="339">
@@ -6217,7 +6213,7 @@
         <v>683</v>
       </c>
       <c r="C339" s="4">
-        <v>454</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="340">
@@ -6228,7 +6224,7 @@
         <v>685</v>
       </c>
       <c r="C340" s="4">
-        <v>404</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="341">
@@ -6239,7 +6235,7 @@
         <v>687</v>
       </c>
       <c r="C341" s="4">
-        <v>307</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="342">
@@ -6250,7 +6246,7 @@
         <v>689</v>
       </c>
       <c r="C342" s="4">
-        <v>158</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343">
@@ -6261,7 +6257,7 @@
         <v>691</v>
       </c>
       <c r="C343" s="4">
-        <v>379</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="344">
@@ -6269,21 +6265,21 @@
         <v>692</v>
       </c>
       <c r="B344" s="0" t="s">
-        <v>693</v>
+        <v>323</v>
       </c>
       <c r="C344" s="4">
-        <v>286</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="B345" s="0" t="s">
         <v>694</v>
       </c>
-      <c r="B345" s="0" t="s">
-        <v>325</v>
-      </c>
       <c r="C345" s="4">
-        <v>828</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="346">
@@ -6294,7 +6290,7 @@
         <v>696</v>
       </c>
       <c r="C346" s="4">
-        <v>320</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="347">
@@ -6305,7 +6301,7 @@
         <v>698</v>
       </c>
       <c r="C347" s="4">
-        <v>722</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="348">
@@ -6316,7 +6312,7 @@
         <v>700</v>
       </c>
       <c r="C348" s="4">
-        <v>307</v>
+        <v>5</v>
       </c>
     </row>
     <row r="349">
@@ -6327,7 +6323,7 @@
         <v>702</v>
       </c>
       <c r="C349" s="4">
-        <v>1938</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="350">
@@ -6338,7 +6334,7 @@
         <v>704</v>
       </c>
       <c r="C350" s="4">
-        <v>289</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="351">
@@ -6349,7 +6345,7 @@
         <v>706</v>
       </c>
       <c r="C351" s="4">
-        <v>286</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="352">
@@ -6357,21 +6353,21 @@
         <v>707</v>
       </c>
       <c r="B352" s="0" t="s">
-        <v>708</v>
+        <v>55</v>
       </c>
       <c r="C352" s="4">
-        <v>469</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="B353" s="0" t="s">
         <v>709</v>
       </c>
-      <c r="B353" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="C353" s="4">
-        <v>277</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="354">
@@ -6382,7 +6378,7 @@
         <v>711</v>
       </c>
       <c r="C354" s="4">
-        <v>298</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="355">
@@ -6393,7 +6389,7 @@
         <v>713</v>
       </c>
       <c r="C355" s="4">
-        <v>405</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="356">
@@ -6404,7 +6400,7 @@
         <v>715</v>
       </c>
       <c r="C356" s="4">
-        <v>370</v>
+        <v>6</v>
       </c>
     </row>
     <row r="357">
@@ -6415,7 +6411,7 @@
         <v>717</v>
       </c>
       <c r="C357" s="4">
-        <v>345</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="358">
@@ -6426,7 +6422,7 @@
         <v>719</v>
       </c>
       <c r="C358" s="4">
-        <v>406</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="359">
@@ -6437,7 +6433,7 @@
         <v>721</v>
       </c>
       <c r="C359" s="4">
-        <v>375</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="360">
@@ -6448,7 +6444,7 @@
         <v>723</v>
       </c>
       <c r="C360" s="4">
-        <v>444</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="361">
@@ -6459,7 +6455,7 @@
         <v>725</v>
       </c>
       <c r="C361" s="4">
-        <v>358</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="362">
@@ -6470,7 +6466,7 @@
         <v>727</v>
       </c>
       <c r="C362" s="4">
-        <v>329</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="363">
@@ -6481,7 +6477,7 @@
         <v>729</v>
       </c>
       <c r="C363" s="4">
-        <v>3152</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="364">
@@ -6492,7 +6488,7 @@
         <v>731</v>
       </c>
       <c r="C364" s="4">
-        <v>209</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="365">
@@ -6503,7 +6499,7 @@
         <v>733</v>
       </c>
       <c r="C365" s="4">
-        <v>212</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="366">
@@ -6514,7 +6510,7 @@
         <v>735</v>
       </c>
       <c r="C366" s="4">
-        <v>234</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="367">
@@ -6525,7 +6521,7 @@
         <v>737</v>
       </c>
       <c r="C367" s="4">
-        <v>393</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="368">
@@ -6536,7 +6532,7 @@
         <v>739</v>
       </c>
       <c r="C368" s="4">
-        <v>298</v>
+        <v>5</v>
       </c>
     </row>
     <row r="369">
@@ -6547,7 +6543,7 @@
         <v>741</v>
       </c>
       <c r="C369" s="4">
-        <v>417</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="370">
@@ -6558,7 +6554,7 @@
         <v>743</v>
       </c>
       <c r="C370" s="4">
-        <v>216</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="371">
@@ -6569,7 +6565,7 @@
         <v>745</v>
       </c>
       <c r="C371" s="4">
-        <v>412</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="372">
@@ -6580,7 +6576,7 @@
         <v>747</v>
       </c>
       <c r="C372" s="4">
-        <v>306</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="373">
@@ -6591,7 +6587,7 @@
         <v>749</v>
       </c>
       <c r="C373" s="4">
-        <v>302</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="374">
@@ -6602,7 +6598,7 @@
         <v>751</v>
       </c>
       <c r="C374" s="4">
-        <v>338</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="375">
@@ -6613,7 +6609,7 @@
         <v>753</v>
       </c>
       <c r="C375" s="4">
-        <v>180</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="376">
@@ -6624,7 +6620,7 @@
         <v>755</v>
       </c>
       <c r="C376" s="4">
-        <v>247</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="377">
@@ -6635,7 +6631,7 @@
         <v>757</v>
       </c>
       <c r="C377" s="4">
-        <v>610</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="378">
@@ -6646,7 +6642,7 @@
         <v>759</v>
       </c>
       <c r="C378" s="4">
-        <v>363</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="379">
@@ -6657,7 +6653,7 @@
         <v>761</v>
       </c>
       <c r="C379" s="4">
-        <v>202</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="380">
@@ -6668,7 +6664,7 @@
         <v>763</v>
       </c>
       <c r="C380" s="4">
-        <v>234</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="381">
@@ -6679,7 +6675,7 @@
         <v>765</v>
       </c>
       <c r="C381" s="4">
-        <v>154</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="382">
@@ -6690,7 +6686,7 @@
         <v>767</v>
       </c>
       <c r="C382" s="4">
-        <v>493</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="383">
@@ -6701,18 +6697,7 @@
         <v>769</v>
       </c>
       <c r="C383" s="4">
-        <v>2210</v>
-      </c>
-    </row>
-    <row r="384">
-      <c r="A384" s="0" t="s">
-        <v>770</v>
-      </c>
-      <c r="B384" s="0" t="s">
-        <v>771</v>
-      </c>
-      <c r="C384" s="4">
-        <v>219</v>
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>